<commit_message>
feature: testing result appear
</commit_message>
<xml_diff>
--- a/output_sandbox.xlsx
+++ b/output_sandbox.xlsx
@@ -458,354 +458,354 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
-        <v>44901</v>
+        <v>43781</v>
       </c>
       <c r="B2" t="n">
-        <v>102</v>
+        <v>2550</v>
       </c>
       <c r="C2" t="n">
-        <v>2865600</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="n">
-        <v>44902</v>
+        <v>43782</v>
       </c>
       <c r="B3" t="n">
-        <v>97</v>
+        <v>2550</v>
       </c>
       <c r="C3" t="n">
-        <v>6235300</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="n">
-        <v>44903</v>
+        <v>43783</v>
       </c>
       <c r="B4" t="n">
-        <v>102</v>
+        <v>2550</v>
       </c>
       <c r="C4" t="n">
-        <v>9217000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="n">
-        <v>44904</v>
+        <v>43784</v>
       </c>
       <c r="B5" t="n">
-        <v>100</v>
+        <v>2550</v>
       </c>
       <c r="C5" t="n">
-        <v>3753800</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="n">
-        <v>44907</v>
+        <v>43787</v>
       </c>
       <c r="B6" t="n">
-        <v>100</v>
+        <v>2550</v>
       </c>
       <c r="C6" t="n">
-        <v>596400</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="n">
-        <v>44908</v>
+        <v>43788</v>
       </c>
       <c r="B7" t="n">
-        <v>97</v>
+        <v>2550</v>
       </c>
       <c r="C7" t="n">
-        <v>4065100</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="n">
-        <v>44909</v>
+        <v>43789</v>
       </c>
       <c r="B8" t="n">
-        <v>94</v>
+        <v>2550</v>
       </c>
       <c r="C8" t="n">
-        <v>3040100</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="n">
-        <v>44910</v>
+        <v>43790</v>
       </c>
       <c r="B9" t="n">
-        <v>93</v>
+        <v>2550</v>
       </c>
       <c r="C9" t="n">
-        <v>4081700</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="n">
-        <v>44911</v>
+        <v>43791</v>
       </c>
       <c r="B10" t="n">
-        <v>94</v>
+        <v>2550</v>
       </c>
       <c r="C10" t="n">
-        <v>2078400</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="n">
-        <v>44914</v>
+        <v>43794</v>
       </c>
       <c r="B11" t="n">
-        <v>95</v>
+        <v>2550</v>
       </c>
       <c r="C11" t="n">
-        <v>11709900</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="n">
-        <v>44915</v>
+        <v>43795</v>
       </c>
       <c r="B12" t="n">
-        <v>95</v>
+        <v>2550</v>
       </c>
       <c r="C12" t="n">
-        <v>2949200</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="2" t="n">
-        <v>44916</v>
+        <v>43796</v>
       </c>
       <c r="B13" t="n">
-        <v>95</v>
+        <v>2550</v>
       </c>
       <c r="C13" t="n">
-        <v>1379800</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="2" t="n">
-        <v>44917</v>
+        <v>43797</v>
       </c>
       <c r="B14" t="n">
-        <v>96</v>
+        <v>2550</v>
       </c>
       <c r="C14" t="n">
-        <v>5115600</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="2" t="n">
-        <v>44918</v>
+        <v>43798</v>
       </c>
       <c r="B15" t="n">
-        <v>94</v>
+        <v>2550</v>
       </c>
       <c r="C15" t="n">
-        <v>2107200</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="2" t="n">
-        <v>44921</v>
+        <v>43801</v>
       </c>
       <c r="B16" t="n">
-        <v>94</v>
+        <v>2550</v>
       </c>
       <c r="C16" t="n">
-        <v>1339900</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="2" t="n">
-        <v>44922</v>
+        <v>43802</v>
       </c>
       <c r="B17" t="n">
-        <v>94</v>
+        <v>2550</v>
       </c>
       <c r="C17" t="n">
-        <v>2718800</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="2" t="n">
-        <v>44923</v>
+        <v>43803</v>
       </c>
       <c r="B18" t="n">
-        <v>97</v>
+        <v>2550</v>
       </c>
       <c r="C18" t="n">
-        <v>5000000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="2" t="n">
-        <v>44924</v>
+        <v>43804</v>
       </c>
       <c r="B19" t="n">
-        <v>94</v>
+        <v>2550</v>
       </c>
       <c r="C19" t="n">
-        <v>21467800</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="2" t="n">
-        <v>44925</v>
+        <v>43805</v>
       </c>
       <c r="B20" t="n">
-        <v>92</v>
+        <v>2550</v>
       </c>
       <c r="C20" t="n">
-        <v>2665100</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="2" t="n">
-        <v>44928</v>
+        <v>43808</v>
       </c>
       <c r="B21" t="n">
-        <v>90</v>
+        <v>2550</v>
       </c>
       <c r="C21" t="n">
-        <v>1336900</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="2" t="n">
-        <v>44929</v>
+        <v>43809</v>
       </c>
       <c r="B22" t="n">
-        <v>90</v>
+        <v>2550</v>
       </c>
       <c r="C22" t="n">
-        <v>2625300</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="2" t="n">
-        <v>44930</v>
+        <v>43810</v>
       </c>
       <c r="B23" t="n">
-        <v>90</v>
+        <v>2550</v>
       </c>
       <c r="C23" t="n">
-        <v>614100</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="2" t="n">
-        <v>44931</v>
+        <v>43811</v>
       </c>
       <c r="B24" t="n">
-        <v>85</v>
+        <v>2550</v>
       </c>
       <c r="C24" t="n">
-        <v>1982300</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="2" t="n">
-        <v>44932</v>
+        <v>43812</v>
       </c>
       <c r="B25" t="n">
-        <v>90</v>
+        <v>2550</v>
       </c>
       <c r="C25" t="n">
-        <v>2509300</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="2" t="n">
-        <v>44935</v>
+        <v>43815</v>
       </c>
       <c r="B26" t="n">
-        <v>89</v>
+        <v>2550</v>
       </c>
       <c r="C26" t="n">
-        <v>1311900</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="2" t="n">
-        <v>44936</v>
+        <v>43816</v>
       </c>
       <c r="B27" t="n">
-        <v>85</v>
+        <v>2550</v>
       </c>
       <c r="C27" t="n">
-        <v>2386900</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="2" t="n">
-        <v>44937</v>
+        <v>43817</v>
       </c>
       <c r="B28" t="n">
-        <v>86</v>
+        <v>2550</v>
       </c>
       <c r="C28" t="n">
-        <v>1094200</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="2" t="n">
-        <v>44938</v>
+        <v>43818</v>
       </c>
       <c r="B29" t="n">
-        <v>86</v>
+        <v>2550</v>
       </c>
       <c r="C29" t="n">
-        <v>431700</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="2" t="n">
-        <v>44939</v>
+        <v>43819</v>
       </c>
       <c r="B30" t="n">
-        <v>86</v>
+        <v>2550</v>
       </c>
       <c r="C30" t="n">
-        <v>410300</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="2" t="n">
-        <v>44942</v>
+        <v>43822</v>
       </c>
       <c r="B31" t="n">
-        <v>86</v>
+        <v>2550</v>
       </c>
       <c r="C31" t="n">
-        <v>2862000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="2" t="n">
-        <v>44943</v>
+        <v>43825</v>
       </c>
       <c r="B32" t="n">
-        <v>86</v>
+        <v>2550</v>
       </c>
       <c r="C32" t="n">
-        <v>2211900</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="2" t="n">
-        <v>44944</v>
+        <v>43826</v>
       </c>
       <c r="B33" t="n">
-        <v>87</v>
+        <v>2550</v>
       </c>
       <c r="C33" t="n">
-        <v>844400</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>